<commit_message>
integrated upload button and validation to Create Screen with Crlist.csv file
</commit_message>
<xml_diff>
--- a/ITT_Integrated_Sep_17/cr_list_entry.xlsx
+++ b/ITT_Integrated_Sep_17/cr_list_entry.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +487,7 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Created on</t>
+          <t xml:space="preserve">   Created    on</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -518,17 +518,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Analysis</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Analysis</t>
+          <t>Built</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Camera</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -544,17 +544,17 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>15.09.2020, 09:10:43</t>
+          <t>17.09.2020, 16:38:34</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>16.09.2020, 16:57:42</t>
+          <t>17.09.2020, 16:38:34</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>['201101', 'Unable to set volume in stereo case', '', 'Swetha', 'Analysis', 'Analysis', 'Camera', 'Bug', '', 'b1', '15.09.2020, 09:10:43', '16.09.2020, 16:57:42', "['201101', 'Unable to set volume in stereo case', '', 'Swetha', 'Open', 'Open', 'Audio', 'Bug', '', 'b1', '15.09.2020, 09:10:43', '15.09.2020, 09:10:43', '', '201101', 'Unable to set volume in stereo case', '', 'Swetha', 'Analysis', 'Analysis', 'Camera', 'Bug', '', 'b1', '15.09.2020, 09:10:43', '16.09.2020, 16:57:42', ' ']", '201101', 'Unable to set volume in stereo case', '', 'Swetha', 'Analysis', 'Analysis', 'Camera', 'Bug', '', 'b1', '15.09.2020, 09:10:43', '16.09.2020, 16:57:42', ' ']</t>
+          <t>['Created by Swetha on18.09.2020, 16:38:34']</t>
         </is>
       </c>
     </row>
@@ -564,32 +564,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Delay in capture</t>
+          <t>Delay in capturing video</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Delay in capturing video.</t>
+          <t>Delay in capturing video</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Pavani</t>
+          <t>pavani</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Analysis</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Analysis</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Camera</t>
+          <t>Video</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -600,22 +600,22 @@
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
-          <t>b2</t>
+          <t>b1</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>16.09.2020, 15:06:10</t>
+          <t>18.09.2020, 16:38:34</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>16.09.2020, 15:06:10</t>
+          <t>18.09.2020, 16:52:43</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>['201102', 'Delay in capture', 'Delay in capturing video.', 'Pavani', 'Open', 'Open', 'Camera', 'Bug', '', 'b2', '16.09.2020, 15:06:10', '16.09.2020, 15:06:10', ' ']</t>
+          <t>["['Created by pavani on 18.09.2020, 16:38:34']", 'pavani', ' changed CR state to Analysis and SI state is changed to Analysis', 'changed domain to Video', ' changed si state to Analysis and CR state is changed to Analysis', 'on', '18.09.2020, 16:52:43']</t>
         </is>
       </c>
     </row>
@@ -625,17 +625,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Blacklisting cr</t>
+          <t>Delay in capture</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Blacking cr's</t>
+          <t>Delay in capture</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Tulasi</t>
+          <t>pavani</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Video</t>
+          <t>Camera</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -666,17 +666,17 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>16.09.2020, 15:09:52</t>
+          <t>18.09.2020, 16:43:04</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>16.09.2020, 15:09:52</t>
+          <t>18.09.2020, 16:43:04</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>['201103', 'Blacklisting cr', "Blacking cr's", 'Tulasi', 'Open', 'Open', 'Video', 'Bug', '', 'b2', '16.09.2020, 15:09:52', '16.09.2020, 15:09:52', ' ']</t>
+          <t>['Created by pavanion18.09.2020, 16:43:04']</t>
         </is>
       </c>
     </row>
@@ -686,32 +686,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Test application not working for some audio formats</t>
+          <t>Blacklisting</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>for samplefile with size 10kb</t>
+          <t>Blacklisting</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Tulasi</t>
+          <t>pavani</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Analysis</t>
+          <t>Open</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Analysis</t>
+          <t>Open</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Camera</t>
+          <t>Audio</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -722,22 +722,22 @@
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
-          <t>b1</t>
+          <t>b3</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>16.09.2020, 17:54:49</t>
+          <t>18.09.2020, 16:43:57</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>16.09.2020, 17:57:50</t>
+          <t>18.09.2020, 16:43:57</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>['201104', 'Test application not working for some audio formats', 'for samplefile with size 10kb', 'Tulasi', 'Analysis', 'Analysis', 'Camera', 'Bug', '', 'b1', '16.09.2020, 17:54:49', '16.09.2020, 17:57:50', '[\'201104\', \'Test application not working for some audio formats\', \'for samplefile with size 10kb\', \'Tulasi\', \'Analysis\', \'Analysis\', \'Camera\', \'Bug\', \'\', \'b1\', \'16.09.2020, 17:54:49\', \'16.09.2020, 17:57:50\', \'[\\\'201104\\\', \\\'Test application not working for some audio formats\\\', \\\'for samplefile\\\', \\\'Tulasi\\\', \\\'Open\\\', \\\'Open\\\', \\\'Audio\\\', \\\'Bug\\\', \\\'\\\', \\\'b1\\\', \\\'16.09.2020, 17:54:49\\\', \\\'16.09.2020, 17:54:49\\\', "[\\\'201104\\\', \\\'Test application not working for some audio formats\\\', \\\'for samplefile\\\', \\\'Tulasi\\\', \\\'Open\\\', \\\'Open\\\', \\\'Audio\\\', \\\'Bug\\\', \\\'\\\', \\\'b1\\\', \\\'16.09.2020, 17:54:49\\\', \\\'16.09.2020, 17:54:49\\\', \\\' \\\']", \\\'201104\\\', \\\'Test application not working for some audio formats\\\', \\\'for samplefile with size 10kb\\\', \\\'Tulasi\\\', \\\'Analysis\\\', \\\'Analysis\\\', \\\'Camera\\\', \\\'Bug\\\', \\\'\\\', \\\'b1\\\', \\\'16.09.2020, 17:54:49\\\', \\\'16.09.2020, 17:57:50\\\', \\\' \\\']\', \'201104\', \'Test application not working for some audio formats\', \'for samplefile with size 10kb\', \'Tulasi\', \'Analysis\', \'Analysis\', \'Camera\', \'Bug\', \'\', \'b1\', \'16.09.2020, 17:54:49\', \'16.09.2020, 17:57:50\', \' \']', '201104', 'Test application not working for some audio formats', 'for samplefile with size 10kb', 'Tulasi', 'Analysis', 'Analysis', 'Camera', 'Bug', '', 'b1', '16.09.2020, 17:54:49', '16.09.2020, 17:57:50', ' ']</t>
+          <t>['Created by pavanion18.09.2020, 16:43:57']</t>
         </is>
       </c>
     </row>
@@ -747,62 +747,867 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>audio getting glich</t>
+          <t>Test application not working for some audio formats</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>sample file getting click at ten sec</t>
+          <t>Test application not working for some audio formats</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>tulasi</t>
+          <t>pavani</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>In-progress</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Audio</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>https://github.com/ts-issue-tracker/Issue_Tracker/tree/27Aug</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>b1</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:45:37</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:57:20</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>['[\'["[\\\'Created by pavanion18.09.2020, 16:45:37\\\']", \\\'pavani\\\', \\\' changed CR state to Analysis and SI state is changed to Analysis\\\', \\\' changed si state to Analysis and CR state is changed to Analysis\\\', \\\'on\\\', \\\'18.09.2020, 16:56:12\\\']\', \'pavani\', \' changed CR state to In-progress and SI state is changed to Fix\', \' changed si state to Fix and CR state is changed to In-progress\', \'on\', \'18.09.2020, 16:56:24\']', 'pavani', ' added git/gerrit id: https://github.com/ts-issue-tracker/Issue_Tracker/tree/27Aug', 'on', '18.09.2020, 16:57:20']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>201106</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Blacklisting</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Blacklisting</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Open</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Open</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Blacklisting</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:46:16</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:46:16</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>['Created by pavanion18.09.2020, 16:46:16']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>201107</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>blacklisting</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>blacklisting</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Reopen</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Built</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>Audio</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Blacklisting</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>https://github.com/ts-issue-tracker/Issue_Tracker/tree/31Aug</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:46:47</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:58:17</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>['[\'["[\\\'Created by pavanion18.09.2020, 16:46:47\\\']", \\\'pavani\\\', \\\' changed CR state to Analysis and SI state is changed to Analysis\\\', \\\' changed si state to Analysis and CR state is changed to Analysis\\\', \\\'on\\\', \\\'18.09.2020, 16:57:07\\\']\', \'pavani\', \' changed CR state to In-progress and SI state is changed to Fix\', \' changed si state to Fix and CR state is changed to In-progress\', \'on\', \'18.09.2020, 16:57:48\']', 'pavani', ' added git/gerrit id: https://github.com/ts-issue-tracker/Issue_Tracker/tree/31Aug', ' changed CR state to Reopen and SI state is changed to Built', ' changed si state to Built and CR state is changed to Reopen', 'on', '18.09.2020, 16:58:17']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>201108</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Front camera is not getting  opened</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Front camera is not getting  opened</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:47:27</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:59:02</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 16:47:27']", 'pavani', ' changed CR state to Analysis and SI state is changed to Analysis', ' changed si state to Analysis and CR state is changed to Analysis', 'on', '18.09.2020, 16:59:02']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>201109</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>HD format selection is not happening</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>HD format selection is not happening</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
         <is>
           <t>Bug</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr">
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>b3</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:47:53</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:59:38</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>['[\'["[\\\'Created by pavanion18.09.2020, 16:47:53\\\']", \\\'pavani\\\', \\\' changed CR state to Analysis and SI state is changed to Analysis\\\', \\\' changed si state to Analysis and CR state is changed to Analysis\\\', \\\'on\\\', \\\'18.09.2020, 16:59:11\\\']\', \'pavani\', \' changed CR state to In-progress and SI state is changed to Fix\', \' changed si state to Fix and CR state is changed to In-progress\', \'on\', \'18.09.2020, 16:59:27\']', 'pavani', ' changed CR state to Closed and SI state is changed to Fix', ' changed si state to Fix and CR state is changed to Closed', 'on', '18.09.2020, 16:59:38']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>201110</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Audio not supporting for dobly DTS format</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Audio not supporting for dobly DTS format</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Audio</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:48:18</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:00:13</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 16:48:18']", 'pavani', 'on', '18.09.2020, 17:00:13']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>201111</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>No audio while playing video</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>No audio while playing video</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>In-progress</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>https://github.com/ts-issue-tracker/Issue_Tracker/tree/Sep-1-Folders</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
         <is>
           <t>b1</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>17.09.2020, 15:49:35</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>17.09.2020, 15:49:35</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>['201105', 'audio getting glich', 'sample file getting click at ten sec', 'tulasi', 'Open', 'Open', 'Audio', 'Bug', '', 'b1', '17.09.2020, 15:49:35', '17.09.2020, 15:49:35', ' ']</t>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:48:40</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:00:37</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>['["[\'Created by pavanion18.09.2020, 16:48:40\']", \'pavani\', \' changed CR state to Analysis and SI state is changed to Analysis\', \' changed si state to Analysis and CR state is changed to Analysis\', \'on\', \'18.09.2020, 17:00:28\']', 'pavani', ' changed CR state to In-progress and SI state is changed to Fix', ' changed si state to Fix and CR state is changed to In-progress', 'on', '18.09.2020, 17:00:37']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>201112</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>blacklisting</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>blacklisting</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Blacklisting</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:49:29</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:01:09</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 16:49:29']", 'pavani', ' changed CR state to Analysis and SI state is changed to Analysis', ' changed si state to Analysis and CR state is changed to Analysis', 'on', '18.09.2020, 17:01:09']</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>201113</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>camera shuting off after 10mins</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>camera shuting off after 10mins</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>b1</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:49:52</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:01:21</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 16:49:52']", 'pavani', 'on', '18.09.2020, 17:01:21']</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>201114</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>unable to hear volume from earphones</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>unable to hear volume from earphones</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>In-progress</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Fix</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Audio</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Bug</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:50:55</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:01:45</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>['["[\'Created by pavanion18.09.2020, 16:50:55\']", \'pavani\', \' changed CR state to Analysis and SI state is changed to Analysis\', \' changed si state to Analysis and CR state is changed to Analysis\', \'on\', \'18.09.2020, 17:01:36\']', 'pavani', ' changed CR state to In-progress and SI state is changed to Fix', ' changed si state to Fix and CR state is changed to In-progress', 'on', '18.09.2020, 17:01:45']</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>201115</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>blur image while recording video</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>blur image while recording video</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Bug</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>18.09.2020, 16:51:37</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:01:56</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 16:51:37']", 'pavani', ' changed CR state to Analysis and SI state is changed to Analysis', ' changed si state to Analysis and CR state is changed to Analysis', 'on', '18.09.2020, 17:01:56']</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>201116</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Delay while recording video</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Delay while recording video</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Analysis</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Internal</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>b1</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:02:49</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:03:40</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 17:02:49']", 'pavani', ' changed CR state to Analysis and SI state is changed to Analysis', ' changed description to Delay while recording video', ' changed issue type to Internal because changed from bug to internal', ' changed si state to Analysis and CR state is changed to Analysis', 'on', '18.09.2020, 17:03:40']</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>201117</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>audio playback issue</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>audio playback issue</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Audio</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Bug</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>b1</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:08:18</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:08:53</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>["['Created by pavanion18.09.2020, 17:08:18']", 'pavani', ' changed issue type to Bug because changed', 'on', '18.09.2020, 17:08:53']</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>201118</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">blacklisting </t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>blacklisting</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>pavani</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Bug</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>b2</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:09:06</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>18.09.2020, 17:09:06</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>['Created by pavanion18.09.2020, 17:09:06']</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>